<commit_message>
Fixed date formats in test spreadsheets
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/data-contracts/EOHHS-075-09302020-bad_proj_id-v1.xlsx
+++ b/tests/server/fixtures/data-contracts/EOHHS-075-09302020-bad_proj_id-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/tests/server/fixtures/data-contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D86017B-1AE7-DF4F-9453-A3DED952D2FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF54F3D-1705-3E46-98AC-1533C1E38034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certification" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="346">
   <si>
     <t>Certification</t>
   </si>
@@ -1663,7 +1663,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2089,9 +2091,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -13495,7 +13495,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>